<commit_message>
committing testng.xml for parallel execution
</commit_message>
<xml_diff>
--- a/uiautomation/src/main/java/hybridFramework/uiautomation/data/Testdata1.xlsx
+++ b/uiautomation/src/main/java/hybridFramework/uiautomation/data/Testdata1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Username</t>
   </si>
@@ -64,6 +64,81 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>selectday</t>
+  </si>
+  <si>
+    <t>selectmont</t>
+  </si>
+  <si>
+    <t>selectyear</t>
+  </si>
+  <si>
+    <t>addressfirstname</t>
+  </si>
+  <si>
+    <t>addresslastname</t>
+  </si>
+  <si>
+    <t>address1</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>selectstate</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>mobileno</t>
+  </si>
+  <si>
+    <t>addressref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sushant </t>
+  </si>
+  <si>
+    <t>Jain</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>megha</t>
+  </si>
+  <si>
+    <t>jain</t>
+  </si>
+  <si>
+    <t>amsterdam</t>
+  </si>
+  <si>
+    <t>udaipur</t>
+  </si>
+  <si>
+    <t>20345</t>
+  </si>
+  <si>
+    <t>0645072609</t>
+  </si>
+  <si>
+    <t>rajasthan</t>
+  </si>
+  <si>
+    <t>emailid</t>
+  </si>
+  <si>
+    <t>sushant2@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -471,14 +546,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -487,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>